<commit_message>
Fixed bug for single and added 4% case
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -5,15 +5,15 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Retirement\harp.d\HARP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Retirement\MyProject\ARP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F669254-C412-4209-A285-C9FB2887C927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66189719-51B6-42EA-A7ED-3B8A50187780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
   </bookViews>
   <sheets>
-    <sheet name="Spouse 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sam" sheetId="1" r:id="rId1"/>
     <sheet name="Spouse 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -422,7 +422,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -898,7 +898,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Renamed a few files and improved Roth optimizer.
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Retirement\MyProject\ARP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66189719-51B6-42EA-A7ED-3B8A50187780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E62D12-4710-4B85-B5EB-9680494BB4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
+    <workbookView xWindow="16215" yWindow="540" windowWidth="21600" windowHeight="11175" activeTab="1" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
   </bookViews>
   <sheets>
     <sheet name="Sam" sheetId="1" r:id="rId1"/>
-    <sheet name="Spouse 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Casey" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -422,28 +422,28 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.81640625" customWidth="1"/>
-    <col min="2" max="2" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -472,7 +472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2023</v>
       </c>
@@ -485,7 +485,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2024</v>
       </c>
@@ -498,7 +498,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2025</v>
       </c>
@@ -511,7 +511,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2026</v>
       </c>
@@ -524,7 +524,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2027</v>
       </c>
@@ -537,7 +537,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2028</v>
       </c>
@@ -550,7 +550,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2029</v>
       </c>
@@ -563,7 +563,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2030</v>
       </c>
@@ -576,7 +576,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2031</v>
       </c>
@@ -589,7 +589,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2032</v>
       </c>
@@ -602,7 +602,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2033</v>
       </c>
@@ -615,7 +615,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2034</v>
       </c>
@@ -628,7 +628,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2035</v>
       </c>
@@ -641,7 +641,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2036</v>
       </c>
@@ -654,7 +654,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2037</v>
       </c>
@@ -667,7 +667,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2038</v>
       </c>
@@ -680,7 +680,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2039</v>
       </c>
@@ -693,7 +693,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2040</v>
       </c>
@@ -706,7 +706,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2041</v>
       </c>
@@ -719,7 +719,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2042</v>
       </c>
@@ -732,7 +732,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2043</v>
       </c>
@@ -745,7 +745,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2044</v>
       </c>
@@ -758,7 +758,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2045</v>
       </c>
@@ -771,7 +771,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2046</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2047</v>
       </c>
@@ -797,7 +797,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2048</v>
       </c>
@@ -810,7 +810,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2049</v>
       </c>
@@ -823,7 +823,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2050</v>
       </c>
@@ -836,7 +836,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2051</v>
       </c>
@@ -849,7 +849,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2052</v>
       </c>
@@ -862,7 +862,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2053</v>
       </c>
@@ -875,7 +875,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2054</v>
       </c>
@@ -898,24 +898,24 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.1796875" customWidth="1"/>
-    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.453125" customWidth="1"/>
-    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -944,7 +944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2023</v>
       </c>
@@ -957,7 +957,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2024</v>
       </c>
@@ -970,7 +970,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2025</v>
       </c>
@@ -983,7 +983,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2026</v>
       </c>
@@ -996,7 +996,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2027</v>
       </c>
@@ -1009,7 +1009,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2028</v>
       </c>
@@ -1022,7 +1022,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2029</v>
       </c>
@@ -1035,7 +1035,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2030</v>
       </c>
@@ -1048,7 +1048,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2031</v>
       </c>
@@ -1061,7 +1061,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2032</v>
       </c>
@@ -1074,7 +1074,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2033</v>
       </c>
@@ -1087,7 +1087,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2034</v>
       </c>
@@ -1100,7 +1100,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2035</v>
       </c>
@@ -1113,7 +1113,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2036</v>
       </c>
@@ -1126,7 +1126,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2037</v>
       </c>
@@ -1139,7 +1139,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2038</v>
       </c>
@@ -1152,7 +1152,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2039</v>
       </c>
@@ -1165,7 +1165,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2040</v>
       </c>
@@ -1178,7 +1178,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2041</v>
       </c>
@@ -1191,7 +1191,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2042</v>
       </c>
@@ -1204,7 +1204,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2043</v>
       </c>
@@ -1217,7 +1217,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2044</v>
       </c>
@@ -1230,7 +1230,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2045</v>
       </c>
@@ -1243,7 +1243,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2046</v>
       </c>
@@ -1256,7 +1256,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2047</v>
       </c>
@@ -1269,7 +1269,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2048</v>
       </c>
@@ -1282,7 +1282,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2049</v>
       </c>
@@ -1295,7 +1295,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2050</v>
       </c>
@@ -1308,7 +1308,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2051</v>
       </c>
@@ -1321,7 +1321,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2052</v>
       </c>
@@ -1334,7 +1334,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2053</v>
       </c>
@@ -1347,7 +1347,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2054</v>
       </c>
@@ -1360,7 +1360,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2055</v>
       </c>
@@ -1373,7 +1373,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2056</v>
       </c>
@@ -1386,7 +1386,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2057</v>
       </c>

</xml_diff>